<commit_message>
monoplex multiplex comparison real networks
</commit_message>
<xml_diff>
--- a/experiments/real_data_experiments/results/results.xlsx
+++ b/experiments/real_data_experiments/results/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuzne\Documents\ACTIVE_PROJECTS\research\experiments\real_data_experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuzne\Documents\ACTIVE_PROJECTS\research\experiments\real_data_experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71BCB7-9553-4FFC-B35C-34F50B16D9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091E7F62-BA73-490E-8A0F-A6364EE0116A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D3DA8771-1432-4179-AD61-E06224215FC4}"/>
   </bookViews>
@@ -197,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +207,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -668,6 +674,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -987,8 +1032,8 @@
   <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3726,193 +3771,193 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="33" t="s">
+    <row r="83" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="34">
+      <c r="B83" s="56">
         <v>4432</v>
       </c>
-      <c r="C83" s="35">
+      <c r="C83" s="57">
         <v>42</v>
       </c>
-      <c r="D83" s="35">
+      <c r="D83" s="57">
         <f t="shared" si="18"/>
         <v>9.4765342960288802E-3</v>
       </c>
-      <c r="E83" s="35">
+      <c r="E83" s="57">
         <v>4432</v>
       </c>
-      <c r="F83" s="35">
+      <c r="F83" s="57">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="G83" s="34">
+      <c r="G83" s="56">
         <v>5</v>
       </c>
-      <c r="H83" s="35">
+      <c r="H83" s="57">
         <v>48.7</v>
       </c>
-      <c r="I83" s="35">
+      <c r="I83" s="57">
         <v>1961</v>
       </c>
-      <c r="J83" s="35">
+      <c r="J83" s="57">
         <v>1734</v>
       </c>
-      <c r="K83" s="35"/>
-      <c r="L83" s="37" t="s">
+      <c r="K83" s="57"/>
+      <c r="L83" s="58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="39" t="s">
+    <row r="84" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B84" s="40">
+      <c r="B84" s="61">
         <v>4432</v>
       </c>
-      <c r="C84" s="41">
+      <c r="C84" s="62">
         <v>16</v>
       </c>
-      <c r="D84" s="41">
+      <c r="D84" s="62">
         <f t="shared" si="18"/>
         <v>3.6101083032490976E-3</v>
       </c>
-      <c r="E84" s="41">
+      <c r="E84" s="62">
         <v>4344</v>
       </c>
-      <c r="F84" s="41">
+      <c r="F84" s="62">
         <f t="shared" si="19"/>
         <v>0.98014440433213001</v>
       </c>
-      <c r="G84" s="40">
+      <c r="G84" s="61">
         <v>5</v>
       </c>
-      <c r="H84" s="41">
+      <c r="H84" s="62">
         <v>48.7</v>
       </c>
-      <c r="I84" s="41">
+      <c r="I84" s="62">
         <v>1961</v>
       </c>
-      <c r="J84" s="41">
+      <c r="J84" s="62">
         <v>1734</v>
       </c>
-      <c r="K84" s="41"/>
-      <c r="L84" s="43" t="s">
+      <c r="K84" s="62"/>
+      <c r="L84" s="63" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="39" t="s">
+    <row r="85" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B85" s="40">
+      <c r="B85" s="61">
         <v>4432</v>
       </c>
-      <c r="C85" s="41">
+      <c r="C85" s="62">
         <v>12</v>
       </c>
-      <c r="D85" s="41">
+      <c r="D85" s="62">
         <f t="shared" si="18"/>
         <v>2.707581227436823E-3</v>
       </c>
-      <c r="E85" s="41">
+      <c r="E85" s="62">
         <v>4310</v>
       </c>
-      <c r="F85" s="41">
+      <c r="F85" s="62">
         <f t="shared" si="19"/>
         <v>0.97247292418772568</v>
       </c>
-      <c r="G85" s="40">
+      <c r="G85" s="61">
         <v>5</v>
       </c>
-      <c r="H85" s="41">
+      <c r="H85" s="62">
         <v>48.7</v>
       </c>
-      <c r="I85" s="41">
+      <c r="I85" s="62">
         <v>1961</v>
       </c>
-      <c r="J85" s="41">
+      <c r="J85" s="62">
         <v>1734</v>
       </c>
-      <c r="K85" s="41"/>
-      <c r="L85" s="43" t="s">
+      <c r="K85" s="62"/>
+      <c r="L85" s="63" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="39" t="s">
+    <row r="86" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B86" s="40">
+      <c r="B86" s="61">
         <v>4432</v>
       </c>
-      <c r="C86" s="41">
+      <c r="C86" s="62">
         <v>6</v>
       </c>
-      <c r="D86" s="41">
+      <c r="D86" s="62">
         <f t="shared" si="18"/>
         <v>1.3537906137184115E-3</v>
       </c>
-      <c r="E86" s="41">
+      <c r="E86" s="62">
         <v>4286</v>
       </c>
-      <c r="F86" s="41">
+      <c r="F86" s="62">
         <f t="shared" si="19"/>
         <v>0.96705776173285196</v>
       </c>
-      <c r="G86" s="40">
+      <c r="G86" s="61">
         <v>5</v>
       </c>
-      <c r="H86" s="41">
+      <c r="H86" s="62">
         <v>48.7</v>
       </c>
-      <c r="I86" s="41">
+      <c r="I86" s="62">
         <v>1961</v>
       </c>
-      <c r="J86" s="41">
+      <c r="J86" s="62">
         <v>1734</v>
       </c>
-      <c r="K86" s="41"/>
-      <c r="L86" s="43" t="s">
+      <c r="K86" s="62"/>
+      <c r="L86" s="63" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="44" t="s">
+    <row r="87" spans="1:12" s="59" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="45">
+      <c r="B87" s="65">
         <v>4432</v>
       </c>
-      <c r="C87" s="46">
-        <v>0</v>
-      </c>
-      <c r="D87" s="46">
+      <c r="C87" s="66">
+        <v>0</v>
+      </c>
+      <c r="D87" s="66">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E87" s="46">
+      <c r="E87" s="66">
         <v>4274</v>
       </c>
-      <c r="F87" s="46">
+      <c r="F87" s="66">
         <f t="shared" si="19"/>
         <v>0.96435018050541521</v>
       </c>
-      <c r="G87" s="45">
+      <c r="G87" s="65">
         <v>5</v>
       </c>
-      <c r="H87" s="46">
+      <c r="H87" s="66">
         <v>48.7</v>
       </c>
-      <c r="I87" s="46">
+      <c r="I87" s="66">
         <v>1961</v>
       </c>
-      <c r="J87" s="46">
+      <c r="J87" s="66">
         <v>1734</v>
       </c>
-      <c r="K87" s="46"/>
-      <c r="L87" s="48" t="s">
+      <c r="K87" s="66"/>
+      <c r="L87" s="67" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update real networks plots
</commit_message>
<xml_diff>
--- a/experiments/real_data_experiments/results/results.xlsx
+++ b/experiments/real_data_experiments/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuzne\Documents\ACTIVE_PROJECTS\research\experiments\real_data_experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091E7F62-BA73-490E-8A0F-A6364EE0116A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F786EB-1C5B-496C-A35C-7DE0525AB505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D3DA8771-1432-4179-AD61-E06224215FC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="49">
   <si>
     <t>Air_Train</t>
   </si>
@@ -164,7 +164,25 @@
     <t>layers 2-4</t>
   </si>
   <si>
-    <t>CovMulNet19</t>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Neural</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Genetic</t>
   </si>
 </sst>
 </file>
@@ -512,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -529,12 +547,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -565,9 +577,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -673,9 +682,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,16 +709,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1029,11 +1041,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94755FB-9259-4D0E-981D-300B3D3492BC}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
+      <selection pane="bottomLeft" activeCell="M83" sqref="M83:M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,10 +1058,11 @@
     <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
     <col min="10" max="11" width="13.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1086,41 +1099,47 @@
       <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11">
+      <c r="M1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
         <v>69</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>12</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="10">
         <f>C2/B$2</f>
         <v>0.17391304347826086</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>67</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="10">
         <f>E2/B$2</f>
         <v>0.97101449275362317</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="9">
         <v>4</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
@@ -1146,13 +1165,16 @@
       <c r="H3" s="5"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3">
@@ -1178,301 +1200,331 @@
       <c r="H4" s="5"/>
       <c r="I4" s="3"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="K4" s="23"/>
+      <c r="L4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
         <v>69</v>
       </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <f t="shared" si="1"/>
         <v>1.4492753623188406E-2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>4</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="31">
         <v>3896</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="32">
         <v>274</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="32">
         <f>C6/B$6</f>
         <v>7.0328542094455854E-2</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="32">
         <v>2252</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="32">
         <f>E6/B$6</f>
         <v>0.57802874743326493</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="31">
         <v>7</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="37" t="s">
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="M6" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="40">
+    </row>
+    <row r="7" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="37">
         <v>3896</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="38">
         <v>118</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="38">
         <f t="shared" ref="D7:D12" si="2">C7/B$6</f>
         <v>3.0287474332648872E-2</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="38">
         <v>1053</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="38">
         <f t="shared" ref="F7:F12" si="3">E7/B$6</f>
         <v>0.27027720739219713</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="37">
         <v>7</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43" t="s">
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="M7" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="40">
+    </row>
+    <row r="8" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="37">
         <v>3896</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="38">
         <v>69</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="38">
         <f t="shared" si="2"/>
         <v>1.7710472279260779E-2</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="38">
         <v>523</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="38">
         <f t="shared" si="3"/>
         <v>0.13424024640657084</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="37">
         <v>7</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43" t="s">
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="M8" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="40">
+    </row>
+    <row r="9" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="37">
         <v>3896</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="38">
         <v>37</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="38">
         <f t="shared" si="2"/>
         <v>9.4969199178644766E-3</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="38">
         <v>191</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="38">
         <f t="shared" si="3"/>
         <v>4.9024640657084187E-2</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="37">
         <v>7</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="43" t="s">
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="M9" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="40">
+    </row>
+    <row r="10" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="37">
         <v>3896</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="38">
         <v>2</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="38">
         <f t="shared" si="2"/>
         <v>5.1334702258726901E-4</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="38">
         <v>32</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="38">
         <f t="shared" si="3"/>
         <v>8.2135523613963042E-3</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="37">
         <v>7</v>
       </c>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43" t="s">
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="M10" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="40">
+    </row>
+    <row r="11" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="37">
         <v>3896</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="38">
         <v>3</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="38">
         <f t="shared" si="2"/>
         <v>7.7002053388090352E-4</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="38">
         <v>28</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="38">
         <f t="shared" si="3"/>
         <v>7.1868583162217657E-3</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="37">
         <v>7</v>
       </c>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="43" t="s">
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
+      <c r="M11" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="45">
+    </row>
+    <row r="12" spans="1:13" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="42">
         <v>3896</v>
       </c>
-      <c r="C12" s="46">
-        <v>0</v>
-      </c>
-      <c r="D12" s="46">
+      <c r="C12" s="43">
+        <v>0</v>
+      </c>
+      <c r="D12" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="43">
         <v>10</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="43">
         <f t="shared" si="3"/>
         <v>2.5667351129363448E-3</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="42">
         <v>7</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="48" t="s">
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="M12" s="64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="9">
         <v>237</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="10">
         <v>50</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <f>C13/B$13</f>
         <v>0.2109704641350211</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>226</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <f>E13/B$13</f>
         <v>0.95358649789029537</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="9">
         <v>4</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="16" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="M13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="3">
@@ -1498,13 +1550,16 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="17" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="M14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="3">
@@ -1530,77 +1585,86 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="17" t="s">
+      <c r="K15" s="28"/>
+      <c r="L15" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="M15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>237</v>
       </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <f t="shared" si="5"/>
         <v>8.4388185654008432E-3</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="6">
         <v>4</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="20" t="s">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="M16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="9">
         <v>557</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="10">
         <v>114</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="10">
         <f>C17/B$17</f>
         <v>0.20466786355475763</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <v>449</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <f>E17/B$17</f>
         <v>0.80610412926391384</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="9">
         <v>5</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="3">
@@ -1626,13 +1690,16 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="K18" s="25"/>
+      <c r="L18" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="3">
@@ -1658,13 +1725,16 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="K19" s="25"/>
+      <c r="L19" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="3">
@@ -1690,77 +1760,86 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="K20" s="25"/>
+      <c r="L20" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>557</v>
       </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7">
         <f>C21/B$17</f>
         <v>0</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <f>E21/B$17</f>
         <v>1.7953321364452424E-3</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="6">
         <v>5</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="9">
         <v>77</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="10">
         <v>14</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="10">
         <f>C22/B$22</f>
         <v>0.18181818181818182</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="10">
         <v>74</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <f>E22/B$22</f>
         <v>0.96103896103896103</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="9">
         <v>9</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="3">
@@ -1786,13 +1865,16 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+      <c r="K23" s="25"/>
+      <c r="L23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="3">
@@ -1818,13 +1900,16 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="K24" s="25"/>
+      <c r="L24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="3">
@@ -1850,13 +1935,16 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="K25" s="25"/>
+      <c r="L25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="3">
@@ -1882,13 +1970,16 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="K26" s="25"/>
+      <c r="L26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="3">
@@ -1914,13 +2005,16 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="K27" s="25"/>
+      <c r="L27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="3">
@@ -1946,13 +2040,16 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="K28" s="25"/>
+      <c r="L28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="3">
@@ -1978,77 +2075,86 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="K29" s="25"/>
+      <c r="L29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>77</v>
       </c>
-      <c r="C30" s="9">
-        <v>0</v>
-      </c>
-      <c r="D30" s="9">
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>3</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <f t="shared" si="7"/>
         <v>3.896103896103896E-2</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="6">
         <v>9</v>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="9">
         <v>4819</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="10">
         <v>670</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="10">
         <f>C31/B$31</f>
         <v>0.13903299439717784</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="10">
         <v>4710</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="10">
         <f>E31/B$31</f>
         <v>0.97738119941896662</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="9">
         <v>3</v>
       </c>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="3">
@@ -2074,77 +2180,86 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="K32" s="25"/>
+      <c r="L32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="6">
         <v>4819</v>
       </c>
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9">
+      <c r="C33" s="7">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="7">
         <v>2</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <f t="shared" si="9"/>
         <v>4.1502386387217268E-4</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="6">
         <v>3</v>
       </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="9">
         <v>202</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="10">
         <v>26</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="10">
         <f>C34/B34</f>
         <v>0.12871287128712872</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="10">
         <v>97</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="10">
         <f>E34/B34</f>
         <v>0.48019801980198018</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="9">
         <v>3</v>
       </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="16" t="s">
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
+      <c r="M34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="3">
@@ -2170,141 +2285,156 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="17" t="s">
+      <c r="K35" s="28"/>
+      <c r="L35" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
+      <c r="M35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="6">
         <v>202</v>
       </c>
-      <c r="C36" s="9">
-        <v>0</v>
-      </c>
-      <c r="D36" s="9">
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="7">
         <v>2</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36" s="7">
         <f t="shared" si="11"/>
         <v>9.9009900990099011E-3</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="6">
         <v>3</v>
       </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="20" t="s">
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="M36" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="9">
         <v>454</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="10">
         <v>78</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="10">
         <f>C37/B$37</f>
         <v>0.17180616740088106</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="10">
         <v>158</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="10">
         <f>E37/B$37</f>
         <v>0.34801762114537443</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="9">
         <v>2</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="6">
         <v>454</v>
       </c>
-      <c r="C38" s="9">
-        <v>0</v>
-      </c>
-      <c r="D38" s="9">
+      <c r="C38" s="7">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7">
         <f>C38/B$37</f>
         <v>0</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="7">
         <v>2</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="7">
         <f>E38/B$37</f>
         <v>4.4052863436123352E-3</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="6">
         <v>2</v>
       </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="9">
         <v>733</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="10">
         <v>157</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="10">
         <f>C39/B39</f>
         <v>0.21418826739427013</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="10">
         <v>510</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="10">
         <f>E39/B39</f>
         <v>0.69577080491132337</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="9">
         <v>3</v>
       </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="16" t="s">
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
+      <c r="M39" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="3">
@@ -2330,141 +2460,156 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="17" t="s">
+      <c r="K40" s="25"/>
+      <c r="L40" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
+      <c r="M40" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="6">
         <v>733</v>
       </c>
-      <c r="C41" s="9">
-        <v>0</v>
-      </c>
-      <c r="D41" s="9">
+      <c r="C41" s="7">
+        <v>0</v>
+      </c>
+      <c r="D41" s="7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="7">
         <v>4</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41" s="7">
         <f t="shared" si="13"/>
         <v>5.4570259208731242E-3</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="6">
         <v>3</v>
       </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="20" t="s">
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="M41" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B42" s="9">
         <v>24</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="10">
         <v>8</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="10">
         <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="10">
         <v>10</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="10">
         <f t="shared" si="13"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="9">
         <v>2</v>
       </c>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="15" t="s">
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="6">
         <v>24</v>
       </c>
-      <c r="C43" s="9">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9">
+      <c r="C43" s="7">
+        <v>0</v>
+      </c>
+      <c r="D43" s="7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="7">
         <v>1</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43" s="7">
         <f t="shared" si="13"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="6">
         <v>2</v>
       </c>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44" s="9">
         <v>42212</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="10">
         <v>3706</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="10">
         <f>C44/$B$44</f>
         <v>8.7794939827537194E-2</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="10">
         <v>37980</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44" s="10">
         <f>E44/$B$44</f>
         <v>0.89974414858334117</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="9">
         <v>3</v>
       </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="14" t="s">
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="3">
@@ -2490,77 +2635,86 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="15" t="s">
+      <c r="K45" s="25"/>
+      <c r="L45" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="6">
         <v>42212</v>
       </c>
-      <c r="C46" s="9">
-        <v>0</v>
-      </c>
-      <c r="D46" s="9">
+      <c r="C46" s="7">
+        <v>0</v>
+      </c>
+      <c r="D46" s="7">
         <f>C46/$B$44</f>
         <v>0</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="7">
         <v>2</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46" s="7">
         <f>E46/$B$44</f>
         <v>4.7379891973846301E-5</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="6">
         <v>3</v>
       </c>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="9">
         <v>135571</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="10">
         <v>15277</v>
       </c>
-      <c r="D47" s="12">
+      <c r="D47" s="10">
         <f>C47/$B$47</f>
         <v>0.11268634147420908</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="10">
         <v>99925</v>
       </c>
-      <c r="F47" s="12">
+      <c r="F47" s="10">
         <f>E47/$B$47</f>
         <v>0.73706766196310425</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="9">
         <v>3</v>
       </c>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B48" s="3">
@@ -2586,77 +2740,86 @@
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
+      <c r="K48" s="25"/>
+      <c r="L48" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="6">
         <v>135571</v>
       </c>
-      <c r="C49" s="9">
-        <v>0</v>
-      </c>
-      <c r="D49" s="9">
+      <c r="C49" s="7">
+        <v>0</v>
+      </c>
+      <c r="D49" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="7">
         <v>2</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49" s="7">
         <f t="shared" si="15"/>
         <v>1.4752417552426404E-5</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="6">
         <v>3</v>
       </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="9">
         <v>32732</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C50" s="10">
         <v>2925</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D50" s="10">
         <f>C50/B50</f>
         <v>8.9362092142246122E-2</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="10">
         <v>24763</v>
       </c>
-      <c r="F50" s="12">
+      <c r="F50" s="10">
         <f>E50/B50</f>
         <v>0.75653794451912504</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="9">
         <v>3</v>
       </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B51" s="3">
@@ -2682,77 +2845,86 @@
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="15" t="s">
+      <c r="K51" s="25"/>
+      <c r="L51" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="6">
         <v>32732</v>
       </c>
-      <c r="C52" s="9">
-        <v>0</v>
-      </c>
-      <c r="D52" s="9">
+      <c r="C52" s="7">
+        <v>0</v>
+      </c>
+      <c r="D52" s="7">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="7">
         <v>1</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52" s="7">
         <f t="shared" si="17"/>
         <v>3.0551142612733715E-5</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="6">
         <v>3</v>
       </c>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="9">
         <v>40148</v>
       </c>
-      <c r="C53" s="12">
+      <c r="C53" s="10">
         <v>2794</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D53" s="10">
         <f>C53/B53</f>
         <v>6.9592507721430705E-2</v>
       </c>
-      <c r="E53" s="12">
+      <c r="E53" s="10">
         <v>15157</v>
       </c>
-      <c r="F53" s="12">
+      <c r="F53" s="10">
         <f>E53/B53</f>
         <v>0.37752814586031685</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G53" s="9">
         <v>3</v>
       </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="14" t="s">
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B54" s="3">
@@ -2762,14 +2934,14 @@
         <v>6</v>
       </c>
       <c r="D54" s="4">
-        <f t="shared" ref="D54:D91" si="18">C54/B54</f>
+        <f t="shared" ref="D54:D87" si="18">C54/B54</f>
         <v>1.4944704593005878E-4</v>
       </c>
       <c r="E54" s="4">
         <v>14</v>
       </c>
       <c r="F54" s="4">
-        <f t="shared" ref="F54:F91" si="19">E54/B54</f>
+        <f t="shared" ref="F54:F87" si="19">E54/B54</f>
         <v>3.4870977383680382E-4</v>
       </c>
       <c r="G54" s="3">
@@ -2778,77 +2950,86 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="15" t="s">
+      <c r="K54" s="25"/>
+      <c r="L54" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="6">
         <v>40148</v>
       </c>
-      <c r="C55" s="9">
-        <v>0</v>
-      </c>
-      <c r="D55" s="9">
+      <c r="C55" s="7">
+        <v>0</v>
+      </c>
+      <c r="D55" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="7">
         <v>2</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F55" s="7">
         <f t="shared" si="19"/>
         <v>4.9815681976686261E-5</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="6">
         <v>3</v>
       </c>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="11">
+      <c r="B56" s="9">
         <v>438392</v>
       </c>
-      <c r="C56" s="12">
+      <c r="C56" s="10">
         <v>38751</v>
       </c>
-      <c r="D56" s="12">
+      <c r="D56" s="10">
         <f t="shared" si="18"/>
         <v>8.8393492581981425E-2</v>
       </c>
-      <c r="E56" s="12">
+      <c r="E56" s="10">
         <v>189048</v>
       </c>
-      <c r="F56" s="12">
+      <c r="F56" s="10">
         <f t="shared" si="19"/>
         <v>0.43123049690687787</v>
       </c>
-      <c r="G56" s="11">
+      <c r="G56" s="9">
         <v>4</v>
       </c>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="25"/>
-      <c r="L56" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="14" t="s">
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B57" s="3">
@@ -2874,13 +3055,16 @@
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
-      <c r="K57" s="28"/>
-      <c r="L57" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="14" t="s">
+      <c r="K57" s="25"/>
+      <c r="L57" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B58" s="3">
@@ -2906,225 +3090,246 @@
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
-      <c r="K58" s="28"/>
-      <c r="L58" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="15" t="s">
+      <c r="K58" s="25"/>
+      <c r="L58" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="6">
         <v>438392</v>
       </c>
-      <c r="C59" s="9">
-        <v>0</v>
-      </c>
-      <c r="D59" s="9">
+      <c r="C59" s="7">
+        <v>0</v>
+      </c>
+      <c r="D59" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="7">
         <v>1</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="7">
         <f t="shared" si="19"/>
         <v>2.2810635230569901E-6</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="6">
         <v>4</v>
       </c>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="33" t="s">
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B60" s="34">
+      <c r="B60" s="31">
         <v>59</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="32">
         <v>3</v>
       </c>
-      <c r="D60" s="35">
+      <c r="D60" s="32">
         <f t="shared" si="18"/>
         <v>5.0847457627118647E-2</v>
       </c>
-      <c r="E60" s="35">
+      <c r="E60" s="32">
         <v>58</v>
       </c>
-      <c r="F60" s="35">
+      <c r="F60" s="32">
         <f t="shared" si="19"/>
         <v>0.98305084745762716</v>
       </c>
-      <c r="G60" s="34">
+      <c r="G60" s="31">
         <v>4</v>
       </c>
-      <c r="H60" s="35">
+      <c r="H60" s="32">
         <v>6.47</v>
       </c>
-      <c r="I60" s="35">
+      <c r="I60" s="32">
         <v>6.51</v>
       </c>
-      <c r="J60" s="35"/>
-      <c r="K60" s="36"/>
-      <c r="L60" s="37" t="s">
+      <c r="J60" s="32"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="39" t="s">
+      <c r="M60" s="64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="40">
+      <c r="B61" s="37">
         <v>59</v>
       </c>
-      <c r="C61" s="41">
+      <c r="C61" s="38">
         <v>3</v>
       </c>
-      <c r="D61" s="41">
+      <c r="D61" s="38">
         <f t="shared" si="18"/>
         <v>5.0847457627118647E-2</v>
       </c>
-      <c r="E61" s="41">
+      <c r="E61" s="38">
         <v>44</v>
       </c>
-      <c r="F61" s="41">
+      <c r="F61" s="38">
         <f t="shared" si="19"/>
         <v>0.74576271186440679</v>
       </c>
-      <c r="G61" s="40">
+      <c r="G61" s="37">
         <v>4</v>
       </c>
-      <c r="H61" s="41">
+      <c r="H61" s="38">
         <v>6.47</v>
       </c>
-      <c r="I61" s="41">
+      <c r="I61" s="38">
         <v>6.51</v>
       </c>
-      <c r="J61" s="41"/>
-      <c r="K61" s="42"/>
-      <c r="L61" s="43" t="s">
+      <c r="J61" s="38"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="39" t="s">
+      <c r="M61" s="64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="40">
+      <c r="B62" s="37">
         <v>59</v>
       </c>
-      <c r="C62" s="41">
+      <c r="C62" s="38">
         <v>2</v>
       </c>
-      <c r="D62" s="41">
+      <c r="D62" s="38">
         <f t="shared" si="18"/>
         <v>3.3898305084745763E-2</v>
       </c>
-      <c r="E62" s="41">
+      <c r="E62" s="38">
         <v>32</v>
       </c>
-      <c r="F62" s="41">
+      <c r="F62" s="38">
         <f t="shared" si="19"/>
         <v>0.5423728813559322</v>
       </c>
-      <c r="G62" s="40">
+      <c r="G62" s="37">
         <v>4</v>
       </c>
-      <c r="H62" s="41">
+      <c r="H62" s="38">
         <v>6.47</v>
       </c>
-      <c r="I62" s="41">
+      <c r="I62" s="38">
         <v>6.51</v>
       </c>
-      <c r="J62" s="41"/>
-      <c r="K62" s="42"/>
-      <c r="L62" s="43" t="s">
+      <c r="J62" s="38"/>
+      <c r="K62" s="39"/>
+      <c r="L62" s="40" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="49" t="s">
+      <c r="M62" s="64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="50">
+      <c r="B63" s="47">
         <v>59</v>
       </c>
-      <c r="C63" s="51">
-        <v>0</v>
-      </c>
-      <c r="D63" s="51">
+      <c r="C63" s="48">
+        <v>0</v>
+      </c>
+      <c r="D63" s="48">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E63" s="51">
+      <c r="E63" s="48">
         <v>29</v>
       </c>
-      <c r="F63" s="51">
+      <c r="F63" s="48">
         <f t="shared" si="19"/>
         <v>0.49152542372881358</v>
       </c>
-      <c r="G63" s="50">
+      <c r="G63" s="47">
         <v>4</v>
       </c>
-      <c r="H63" s="51">
+      <c r="H63" s="48">
         <v>6.47</v>
       </c>
-      <c r="I63" s="51">
+      <c r="I63" s="48">
         <v>6.51</v>
       </c>
-      <c r="J63" s="51"/>
-      <c r="K63" s="52"/>
-      <c r="L63" s="53" t="s">
+      <c r="J63" s="48"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="21" t="s">
+      <c r="M63" s="64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B64" s="22">
+      <c r="B64" s="19">
         <v>1449</v>
       </c>
-      <c r="C64" s="23">
+      <c r="C64" s="20">
         <v>143</v>
       </c>
-      <c r="D64" s="23">
+      <c r="D64" s="20">
         <f t="shared" si="18"/>
         <v>9.8688750862663904E-2</v>
       </c>
-      <c r="E64" s="23">
+      <c r="E64" s="20">
         <v>442</v>
       </c>
-      <c r="F64" s="23">
+      <c r="F64" s="20">
         <f t="shared" si="19"/>
         <v>0.30503795721187027</v>
       </c>
-      <c r="G64" s="22">
+      <c r="G64" s="19">
         <v>5</v>
       </c>
-      <c r="H64" s="23">
+      <c r="H64" s="20">
         <v>2.94</v>
       </c>
-      <c r="I64" s="23">
+      <c r="I64" s="20">
         <v>2.88</v>
       </c>
-      <c r="J64" s="23"/>
-      <c r="K64" s="26"/>
-      <c r="L64" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="14" t="s">
+      <c r="J64" s="20"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B65" s="3">
@@ -3154,13 +3359,16 @@
         <v>2.88</v>
       </c>
       <c r="J65" s="4"/>
-      <c r="K65" s="28"/>
-      <c r="L65" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="14" t="s">
+      <c r="K65" s="25"/>
+      <c r="L65" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B66" s="3">
@@ -3190,13 +3398,16 @@
         <v>2.88</v>
       </c>
       <c r="J66" s="4"/>
-      <c r="K66" s="28"/>
-      <c r="L66" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="14" t="s">
+      <c r="K66" s="25"/>
+      <c r="L66" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B67" s="3">
@@ -3226,229 +3437,250 @@
         <v>2.88</v>
       </c>
       <c r="J67" s="4"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="15" t="s">
+      <c r="K67" s="25"/>
+      <c r="L67" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="6">
         <v>1449</v>
       </c>
-      <c r="C68" s="9">
-        <v>0</v>
-      </c>
-      <c r="D68" s="9">
+      <c r="C68" s="7">
+        <v>0</v>
+      </c>
+      <c r="D68" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="7">
         <v>1</v>
       </c>
-      <c r="F68" s="9">
+      <c r="F68" s="7">
         <f t="shared" si="19"/>
         <v>6.9013112491373362E-4</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G68" s="6">
         <v>5</v>
       </c>
-      <c r="H68" s="9">
+      <c r="H68" s="7">
         <v>2.94</v>
       </c>
-      <c r="I68" s="9">
+      <c r="I68" s="7">
         <v>2.88</v>
       </c>
-      <c r="J68" s="9"/>
-      <c r="K68" s="29"/>
-      <c r="L68" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="s">
+      <c r="J68" s="7"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B69" s="9">
         <v>33</v>
       </c>
-      <c r="C69" s="12">
+      <c r="C69" s="10">
         <v>1</v>
       </c>
-      <c r="D69" s="12">
+      <c r="D69" s="10">
         <f t="shared" si="18"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="E69" s="12">
+      <c r="E69" s="10">
         <v>3</v>
       </c>
-      <c r="F69" s="12">
+      <c r="F69" s="10">
         <f t="shared" si="19"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="G69" s="11">
+      <c r="G69" s="9">
         <v>2</v>
       </c>
-      <c r="H69" s="12">
+      <c r="H69" s="10">
         <v>0.79</v>
       </c>
-      <c r="I69" s="12">
+      <c r="I69" s="10">
         <v>0.85</v>
       </c>
-      <c r="J69" s="12"/>
-      <c r="K69" s="25"/>
-      <c r="L69" s="16" t="s">
+      <c r="J69" s="10"/>
+      <c r="K69" s="22"/>
+      <c r="L69" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="15" t="s">
+      <c r="M69" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="6">
         <v>33</v>
       </c>
-      <c r="C70" s="9">
-        <v>0</v>
-      </c>
-      <c r="D70" s="9">
+      <c r="C70" s="7">
+        <v>0</v>
+      </c>
+      <c r="D70" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E70" s="7">
         <v>1</v>
       </c>
-      <c r="F70" s="9">
+      <c r="F70" s="7">
         <f t="shared" si="19"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="6">
         <v>2</v>
       </c>
-      <c r="H70" s="9">
+      <c r="H70" s="7">
         <v>0.79</v>
       </c>
-      <c r="I70" s="9">
+      <c r="I70" s="7">
         <v>0.85</v>
       </c>
-      <c r="J70" s="9"/>
-      <c r="K70" s="29"/>
-      <c r="L70" s="20" t="s">
+      <c r="J70" s="7"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="s">
+      <c r="M70" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="9">
         <v>380</v>
       </c>
-      <c r="C71" s="12">
+      <c r="C71" s="10">
         <v>24</v>
       </c>
-      <c r="D71" s="12">
+      <c r="D71" s="10">
         <f t="shared" si="18"/>
         <v>6.3157894736842107E-2</v>
       </c>
-      <c r="E71" s="12">
+      <c r="E71" s="10">
         <v>46</v>
       </c>
-      <c r="F71" s="12">
+      <c r="F71" s="10">
         <f t="shared" si="19"/>
         <v>0.12105263157894737</v>
       </c>
-      <c r="G71" s="11">
+      <c r="G71" s="9">
         <v>2</v>
       </c>
-      <c r="H71" s="12">
+      <c r="H71" s="10">
         <v>1.1599999999999999</v>
       </c>
-      <c r="I71" s="12">
+      <c r="I71" s="10">
         <v>3.14</v>
       </c>
-      <c r="J71" s="12"/>
-      <c r="K71" s="25"/>
-      <c r="L71" s="16" t="s">
+      <c r="J71" s="10"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="15" t="s">
+      <c r="M71" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B72" s="6">
         <v>380</v>
       </c>
-      <c r="C72" s="9">
-        <v>0</v>
-      </c>
-      <c r="D72" s="9">
+      <c r="C72" s="7">
+        <v>0</v>
+      </c>
+      <c r="D72" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E72" s="9">
+      <c r="E72" s="7">
         <v>1</v>
       </c>
-      <c r="F72" s="9">
+      <c r="F72" s="7">
         <f t="shared" si="19"/>
         <v>2.631578947368421E-3</v>
       </c>
-      <c r="G72" s="8">
+      <c r="G72" s="6">
         <v>2</v>
       </c>
-      <c r="H72" s="9">
+      <c r="H72" s="7">
         <v>1.1599999999999999</v>
       </c>
-      <c r="I72" s="9">
+      <c r="I72" s="7">
         <v>3.14</v>
       </c>
-      <c r="J72" s="9"/>
-      <c r="K72" s="29"/>
-      <c r="L72" s="20" t="s">
+      <c r="J72" s="7"/>
+      <c r="K72" s="26"/>
+      <c r="L72" s="17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="10" t="s">
+      <c r="M72" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A73" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="9">
         <v>2147</v>
       </c>
-      <c r="C73" s="12">
+      <c r="C73" s="10">
         <v>408</v>
       </c>
-      <c r="D73" s="12">
+      <c r="D73" s="10">
         <f t="shared" si="18"/>
         <v>0.19003260363297625</v>
       </c>
-      <c r="E73" s="12">
+      <c r="E73" s="10">
         <v>1024</v>
       </c>
-      <c r="F73" s="12">
+      <c r="F73" s="10">
         <f t="shared" si="19"/>
         <v>0.4769445738239404</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G73" s="9">
         <v>3</v>
       </c>
-      <c r="H73" s="12">
+      <c r="H73" s="10">
         <v>2.92</v>
       </c>
-      <c r="I73" s="12">
+      <c r="I73" s="10">
         <v>7.96</v>
       </c>
-      <c r="J73" s="12"/>
-      <c r="K73" s="12"/>
-      <c r="L73" s="16" t="s">
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="14" t="s">
+      <c r="M73" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B74" s="3">
@@ -3479,643 +3711,541 @@
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="17" t="s">
+      <c r="L74" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="15" t="s">
+      <c r="M74" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="6">
         <v>2147</v>
       </c>
-      <c r="C75" s="9">
-        <v>0</v>
-      </c>
-      <c r="D75" s="9">
+      <c r="C75" s="7">
+        <v>0</v>
+      </c>
+      <c r="D75" s="7">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E75" s="9">
+      <c r="E75" s="7">
         <v>2</v>
       </c>
-      <c r="F75" s="9">
+      <c r="F75" s="7">
         <f t="shared" si="19"/>
         <v>9.3153237074988359E-4</v>
       </c>
-      <c r="G75" s="8">
+      <c r="G75" s="6">
         <v>3</v>
       </c>
-      <c r="H75" s="9">
+      <c r="H75" s="7">
         <v>2.92</v>
       </c>
-      <c r="I75" s="9">
+      <c r="I75" s="7">
         <v>7.96</v>
       </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="20" t="s">
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="33" t="s">
+      <c r="M75" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B76" s="34">
+      <c r="B76" s="31">
         <v>4634</v>
       </c>
-      <c r="C76" s="35">
+      <c r="C76" s="32">
         <v>471</v>
       </c>
-      <c r="D76" s="35">
+      <c r="D76" s="32">
         <f t="shared" si="18"/>
         <v>0.10164005179110919</v>
       </c>
-      <c r="E76" s="35">
+      <c r="E76" s="32">
         <v>4571</v>
       </c>
-      <c r="F76" s="35">
+      <c r="F76" s="32">
         <f t="shared" si="19"/>
         <v>0.98640483383685795</v>
       </c>
-      <c r="G76" s="34">
+      <c r="G76" s="31">
         <v>7</v>
       </c>
-      <c r="H76" s="35">
+      <c r="H76" s="32">
         <v>21.81</v>
       </c>
-      <c r="I76" s="35">
+      <c r="I76" s="32">
         <v>11.42</v>
       </c>
-      <c r="J76" s="35"/>
-      <c r="K76" s="35"/>
-      <c r="L76" s="37" t="s">
+      <c r="J76" s="32"/>
+      <c r="K76" s="32"/>
+      <c r="L76" s="34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="39" t="s">
+      <c r="M76" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="40">
+      <c r="B77" s="37">
         <v>4634</v>
       </c>
-      <c r="C77" s="41">
+      <c r="C77" s="38">
         <v>514</v>
       </c>
-      <c r="D77" s="41">
+      <c r="D77" s="38">
         <f t="shared" si="18"/>
         <v>0.11091929218817437</v>
       </c>
-      <c r="E77" s="41">
+      <c r="E77" s="38">
         <v>2624</v>
       </c>
-      <c r="F77" s="41">
+      <c r="F77" s="38">
         <f t="shared" si="19"/>
         <v>0.56624946050927927</v>
       </c>
-      <c r="G77" s="40">
+      <c r="G77" s="37">
         <v>7</v>
       </c>
-      <c r="H77" s="41">
+      <c r="H77" s="38">
         <v>21.81</v>
       </c>
-      <c r="I77" s="41">
+      <c r="I77" s="38">
         <v>11.42</v>
       </c>
-      <c r="J77" s="41"/>
-      <c r="K77" s="41"/>
-      <c r="L77" s="43" t="s">
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+      <c r="L77" s="40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="39" t="s">
+      <c r="M77" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B78" s="40">
+      <c r="B78" s="37">
         <v>4634</v>
       </c>
-      <c r="C78" s="41">
+      <c r="C78" s="38">
         <v>290</v>
       </c>
-      <c r="D78" s="41">
+      <c r="D78" s="38">
         <f t="shared" si="18"/>
         <v>6.2580923608113945E-2</v>
       </c>
-      <c r="E78" s="41">
+      <c r="E78" s="38">
         <v>1259</v>
       </c>
-      <c r="F78" s="41">
+      <c r="F78" s="38">
         <f t="shared" si="19"/>
         <v>0.27168752697453602</v>
       </c>
-      <c r="G78" s="40">
+      <c r="G78" s="37">
         <v>7</v>
       </c>
-      <c r="H78" s="41">
+      <c r="H78" s="38">
         <v>21.81</v>
       </c>
-      <c r="I78" s="41">
+      <c r="I78" s="38">
         <v>11.42</v>
       </c>
-      <c r="J78" s="41"/>
-      <c r="K78" s="41"/>
-      <c r="L78" s="43" t="s">
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="39" t="s">
+      <c r="M78" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B79" s="40">
+      <c r="B79" s="37">
         <v>4634</v>
       </c>
-      <c r="C79" s="41">
+      <c r="C79" s="38">
         <v>139</v>
       </c>
-      <c r="D79" s="41">
+      <c r="D79" s="38">
         <f t="shared" si="18"/>
         <v>2.9995684074233923E-2</v>
       </c>
-      <c r="E79" s="41">
+      <c r="E79" s="38">
         <v>540</v>
       </c>
-      <c r="F79" s="41">
+      <c r="F79" s="38">
         <f t="shared" si="19"/>
         <v>0.11652999568407424</v>
       </c>
-      <c r="G79" s="40">
+      <c r="G79" s="37">
         <v>7</v>
       </c>
-      <c r="H79" s="41">
+      <c r="H79" s="38">
         <v>21.81</v>
       </c>
-      <c r="I79" s="41">
+      <c r="I79" s="38">
         <v>11.42</v>
       </c>
-      <c r="J79" s="41"/>
-      <c r="K79" s="41"/>
-      <c r="L79" s="43" t="s">
+      <c r="J79" s="38"/>
+      <c r="K79" s="38"/>
+      <c r="L79" s="40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="39" t="s">
+      <c r="M79" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B80" s="40">
+      <c r="B80" s="37">
         <v>4634</v>
       </c>
-      <c r="C80" s="41">
+      <c r="C80" s="38">
         <v>23</v>
       </c>
-      <c r="D80" s="41">
+      <c r="D80" s="38">
         <f t="shared" si="18"/>
         <v>4.9633146309883474E-3</v>
       </c>
-      <c r="E80" s="41">
+      <c r="E80" s="38">
         <v>58</v>
       </c>
-      <c r="F80" s="41">
+      <c r="F80" s="38">
         <f t="shared" si="19"/>
         <v>1.2516184721622789E-2</v>
       </c>
-      <c r="G80" s="40">
+      <c r="G80" s="37">
         <v>7</v>
       </c>
-      <c r="H80" s="41">
+      <c r="H80" s="38">
         <v>21.81</v>
       </c>
-      <c r="I80" s="41">
+      <c r="I80" s="38">
         <v>11.42</v>
       </c>
-      <c r="J80" s="41"/>
-      <c r="K80" s="41"/>
-      <c r="L80" s="43" t="s">
+      <c r="J80" s="38"/>
+      <c r="K80" s="38"/>
+      <c r="L80" s="40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="39" t="s">
+      <c r="M80" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B81" s="40">
+      <c r="B81" s="37">
         <v>4634</v>
       </c>
-      <c r="C81" s="41">
+      <c r="C81" s="38">
         <v>2</v>
       </c>
-      <c r="D81" s="41">
+      <c r="D81" s="38">
         <f t="shared" si="18"/>
         <v>4.3159257660768235E-4</v>
       </c>
-      <c r="E81" s="41">
+      <c r="E81" s="38">
         <v>14</v>
       </c>
-      <c r="F81" s="41">
+      <c r="F81" s="38">
         <f t="shared" si="19"/>
         <v>3.0211480362537764E-3</v>
       </c>
-      <c r="G81" s="40">
+      <c r="G81" s="37">
         <v>7</v>
       </c>
-      <c r="H81" s="41">
+      <c r="H81" s="38">
         <v>21.81</v>
       </c>
-      <c r="I81" s="41">
+      <c r="I81" s="38">
         <v>11.42</v>
       </c>
-      <c r="J81" s="41"/>
-      <c r="K81" s="41"/>
-      <c r="L81" s="43" t="s">
+      <c r="J81" s="38"/>
+      <c r="K81" s="38"/>
+      <c r="L81" s="40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="44" t="s">
+      <c r="M81" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B82" s="45">
+      <c r="B82" s="42">
         <v>4634</v>
       </c>
-      <c r="C82" s="46">
-        <v>0</v>
-      </c>
-      <c r="D82" s="46">
+      <c r="C82" s="43">
+        <v>0</v>
+      </c>
+      <c r="D82" s="43">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E82" s="46">
+      <c r="E82" s="43">
         <v>7</v>
       </c>
-      <c r="F82" s="46">
+      <c r="F82" s="43">
         <f t="shared" si="19"/>
         <v>1.5105740181268882E-3</v>
       </c>
-      <c r="G82" s="45">
+      <c r="G82" s="42">
         <v>7</v>
       </c>
-      <c r="H82" s="46">
+      <c r="H82" s="43">
         <v>21.81</v>
       </c>
-      <c r="I82" s="46">
+      <c r="I82" s="43">
         <v>11.42</v>
       </c>
-      <c r="J82" s="46"/>
-      <c r="K82" s="46"/>
-      <c r="L82" s="48" t="s">
+      <c r="J82" s="43"/>
+      <c r="K82" s="43"/>
+      <c r="L82" s="45" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="55" t="s">
+      <c r="M82" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="56">
+      <c r="B83" s="52">
         <v>4432</v>
       </c>
-      <c r="C83" s="57">
+      <c r="C83" s="53">
         <v>42</v>
       </c>
-      <c r="D83" s="57">
+      <c r="D83" s="53">
         <f t="shared" si="18"/>
         <v>9.4765342960288802E-3</v>
       </c>
-      <c r="E83" s="57">
+      <c r="E83" s="53">
         <v>4432</v>
       </c>
-      <c r="F83" s="57">
+      <c r="F83" s="53">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="G83" s="56">
+      <c r="G83" s="52">
         <v>5</v>
       </c>
-      <c r="H83" s="57">
+      <c r="H83" s="53">
         <v>48.7</v>
       </c>
-      <c r="I83" s="57">
+      <c r="I83" s="53">
         <v>1961</v>
       </c>
-      <c r="J83" s="57">
+      <c r="J83" s="53">
         <v>1734</v>
       </c>
-      <c r="K83" s="57"/>
-      <c r="L83" s="58" t="s">
+      <c r="K83" s="53"/>
+      <c r="L83" s="54" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="60" t="s">
+      <c r="M83" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B84" s="61">
+      <c r="B84" s="57">
         <v>4432</v>
       </c>
-      <c r="C84" s="62">
+      <c r="C84" s="58">
         <v>16</v>
       </c>
-      <c r="D84" s="62">
+      <c r="D84" s="58">
         <f t="shared" si="18"/>
         <v>3.6101083032490976E-3</v>
       </c>
-      <c r="E84" s="62">
+      <c r="E84" s="58">
         <v>4344</v>
       </c>
-      <c r="F84" s="62">
+      <c r="F84" s="58">
         <f t="shared" si="19"/>
         <v>0.98014440433213001</v>
       </c>
-      <c r="G84" s="61">
+      <c r="G84" s="57">
         <v>5</v>
       </c>
-      <c r="H84" s="62">
+      <c r="H84" s="58">
         <v>48.7</v>
       </c>
-      <c r="I84" s="62">
+      <c r="I84" s="58">
         <v>1961</v>
       </c>
-      <c r="J84" s="62">
+      <c r="J84" s="58">
         <v>1734</v>
       </c>
-      <c r="K84" s="62"/>
-      <c r="L84" s="63" t="s">
+      <c r="K84" s="58"/>
+      <c r="L84" s="59" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="60" t="s">
+      <c r="M84" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B85" s="61">
+      <c r="B85" s="57">
         <v>4432</v>
       </c>
-      <c r="C85" s="62">
+      <c r="C85" s="58">
         <v>12</v>
       </c>
-      <c r="D85" s="62">
+      <c r="D85" s="58">
         <f t="shared" si="18"/>
         <v>2.707581227436823E-3</v>
       </c>
-      <c r="E85" s="62">
+      <c r="E85" s="58">
         <v>4310</v>
       </c>
-      <c r="F85" s="62">
+      <c r="F85" s="58">
         <f t="shared" si="19"/>
         <v>0.97247292418772568</v>
       </c>
-      <c r="G85" s="61">
+      <c r="G85" s="57">
         <v>5</v>
       </c>
-      <c r="H85" s="62">
+      <c r="H85" s="58">
         <v>48.7</v>
       </c>
-      <c r="I85" s="62">
+      <c r="I85" s="58">
         <v>1961</v>
       </c>
-      <c r="J85" s="62">
+      <c r="J85" s="58">
         <v>1734</v>
       </c>
-      <c r="K85" s="62"/>
-      <c r="L85" s="63" t="s">
+      <c r="K85" s="58"/>
+      <c r="L85" s="59" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="60" t="s">
+      <c r="M85" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B86" s="61">
+      <c r="B86" s="57">
         <v>4432</v>
       </c>
-      <c r="C86" s="62">
+      <c r="C86" s="58">
         <v>6</v>
       </c>
-      <c r="D86" s="62">
+      <c r="D86" s="58">
         <f t="shared" si="18"/>
         <v>1.3537906137184115E-3</v>
       </c>
-      <c r="E86" s="62">
+      <c r="E86" s="58">
         <v>4286</v>
       </c>
-      <c r="F86" s="62">
+      <c r="F86" s="58">
         <f t="shared" si="19"/>
         <v>0.96705776173285196</v>
       </c>
-      <c r="G86" s="61">
+      <c r="G86" s="57">
         <v>5</v>
       </c>
-      <c r="H86" s="62">
+      <c r="H86" s="58">
         <v>48.7</v>
       </c>
-      <c r="I86" s="62">
+      <c r="I86" s="58">
         <v>1961</v>
       </c>
-      <c r="J86" s="62">
+      <c r="J86" s="58">
         <v>1734</v>
       </c>
-      <c r="K86" s="62"/>
-      <c r="L86" s="63" t="s">
+      <c r="K86" s="58"/>
+      <c r="L86" s="59" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" s="59" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="64" t="s">
+      <c r="M86" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="55" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="65">
+      <c r="B87" s="61">
         <v>4432</v>
       </c>
-      <c r="C87" s="66">
-        <v>0</v>
-      </c>
-      <c r="D87" s="66">
+      <c r="C87" s="62">
+        <v>0</v>
+      </c>
+      <c r="D87" s="62">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E87" s="66">
+      <c r="E87" s="62">
         <v>4274</v>
       </c>
-      <c r="F87" s="66">
+      <c r="F87" s="62">
         <f t="shared" si="19"/>
         <v>0.96435018050541521</v>
       </c>
-      <c r="G87" s="65">
+      <c r="G87" s="61">
         <v>5</v>
       </c>
-      <c r="H87" s="66">
+      <c r="H87" s="62">
         <v>48.7</v>
       </c>
-      <c r="I87" s="66">
+      <c r="I87" s="62">
         <v>1961</v>
       </c>
-      <c r="J87" s="66">
+      <c r="J87" s="62">
         <v>1734</v>
       </c>
-      <c r="K87" s="66"/>
-      <c r="L87" s="67" t="s">
+      <c r="K87" s="62"/>
+      <c r="L87" s="63" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A88" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B88" s="11">
-        <v>12658</v>
-      </c>
-      <c r="C88" s="12">
-        <v>279</v>
-      </c>
-      <c r="D88" s="12">
-        <f t="shared" si="18"/>
-        <v>2.2041396745141412E-2</v>
-      </c>
-      <c r="E88" s="12">
-        <v>12658</v>
-      </c>
-      <c r="F88" s="12">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="G88" s="11">
-        <v>4</v>
-      </c>
-      <c r="H88" s="12">
-        <v>5.76</v>
-      </c>
-      <c r="I88" s="12">
-        <v>5.76</v>
-      </c>
-      <c r="J88" s="12"/>
-      <c r="K88" s="12"/>
-      <c r="L88" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B89" s="3">
-        <v>12658</v>
-      </c>
-      <c r="C89" s="4">
-        <v>78</v>
-      </c>
-      <c r="D89" s="4">
-        <f t="shared" si="18"/>
-        <v>6.1621109179965236E-3</v>
-      </c>
-      <c r="E89" s="4">
-        <v>718</v>
-      </c>
-      <c r="F89" s="4">
-        <f t="shared" si="19"/>
-        <v>5.6723021014378261E-2</v>
-      </c>
-      <c r="G89" s="3">
-        <v>4</v>
-      </c>
-      <c r="H89" s="4">
-        <v>5.76</v>
-      </c>
-      <c r="I89" s="4">
-        <v>5.76</v>
-      </c>
-      <c r="J89" s="4"/>
-      <c r="K89" s="4"/>
-      <c r="L89" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A90" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B90" s="3">
-        <v>12658</v>
-      </c>
-      <c r="C90" s="4">
-        <v>6</v>
-      </c>
-      <c r="D90" s="4">
-        <f t="shared" si="18"/>
-        <v>4.7400853215357879E-4</v>
-      </c>
-      <c r="E90" s="4">
-        <v>17</v>
-      </c>
-      <c r="F90" s="4">
-        <f t="shared" si="19"/>
-        <v>1.3430241744351399E-3</v>
-      </c>
-      <c r="G90" s="3">
-        <v>4</v>
-      </c>
-      <c r="H90" s="4">
-        <v>5.76</v>
-      </c>
-      <c r="I90" s="4">
-        <v>5.76</v>
-      </c>
-      <c r="J90" s="4"/>
-      <c r="K90" s="4"/>
-      <c r="L90" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="B91" s="6">
-        <v>12658</v>
-      </c>
-      <c r="C91" s="7">
-        <v>0</v>
-      </c>
-      <c r="D91" s="7">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E91" s="7">
-        <v>1</v>
-      </c>
-      <c r="F91" s="7">
-        <f t="shared" si="19"/>
-        <v>7.9001422025596461E-5</v>
-      </c>
-      <c r="G91" s="6">
-        <v>4</v>
-      </c>
-      <c r="H91" s="7">
-        <v>5.76</v>
-      </c>
-      <c r="I91" s="7">
-        <v>5.76</v>
-      </c>
-      <c r="J91" s="7"/>
-      <c r="K91" s="7"/>
-      <c r="L91" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
+      <c r="M87" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
add citations improve plots add three layered experiment in C++ code
</commit_message>
<xml_diff>
--- a/experiments/real_data_experiments/results/results.xlsx
+++ b/experiments/real_data_experiments/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuzne\Documents\ACTIVE_PROJECTS\research\experiments\real_data_experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F786EB-1C5B-496C-A35C-7DE0525AB505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCDB81E-C19C-4FFA-A93C-74E21F5D02FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D3DA8771-1432-4179-AD61-E06224215FC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
   <si>
     <t>Air_Train</t>
   </si>
@@ -143,18 +143,9 @@
     <t>Bos_Multiplex_Genetic</t>
   </si>
   <si>
-    <t>Celegans_Multiplex_Genetic</t>
-  </si>
-  <si>
-    <t>Drosophila_Multiplex_Genetic</t>
-  </si>
-  <si>
     <t>layer 4 degree</t>
   </si>
   <si>
-    <t>layers 1, 4</t>
-  </si>
-  <si>
     <t>SacchCere_Multiplex_Genetic</t>
   </si>
   <si>
@@ -170,19 +161,13 @@
     <t>Transport</t>
   </si>
   <si>
-    <t>Neural</t>
-  </si>
-  <si>
-    <t>Protein</t>
-  </si>
-  <si>
     <t>Internet</t>
   </si>
   <si>
     <t>Social</t>
   </si>
   <si>
-    <t>Genetic</t>
+    <t>Biological</t>
   </si>
 </sst>
 </file>
@@ -1041,11 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94755FB-9259-4D0E-981D-300B3D3492BC}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M83" sqref="M83:M87"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,13 +1079,13 @@
         <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1135,7 +1120,7 @@
         <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1170,7 +1155,7 @@
         <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1205,7 +1190,7 @@
         <v>25</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1240,7 +1225,7 @@
         <v>25</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -1520,7 +1505,7 @@
         <v>24</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1555,7 +1540,7 @@
         <v>24</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1590,7 +1575,7 @@
         <v>24</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1625,7 +1610,7 @@
         <v>24</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1660,7 +1645,7 @@
         <v>25</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1695,7 +1680,7 @@
         <v>25</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1730,7 +1715,7 @@
         <v>25</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1765,7 +1750,7 @@
         <v>25</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1800,7 +1785,7 @@
         <v>25</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1835,7 +1820,7 @@
         <v>25</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1870,7 +1855,7 @@
         <v>25</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1905,7 +1890,7 @@
         <v>25</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1940,7 +1925,7 @@
         <v>25</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1975,7 +1960,7 @@
         <v>25</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2010,7 +1995,7 @@
         <v>25</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -2045,7 +2030,7 @@
         <v>25</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -2080,7 +2065,7 @@
         <v>25</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2115,7 +2100,7 @@
         <v>25</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2150,7 +2135,7 @@
         <v>25</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2185,7 +2170,7 @@
         <v>25</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2220,7 +2205,7 @@
         <v>25</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -2255,7 +2240,7 @@
         <v>26</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2290,7 +2275,7 @@
         <v>26</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2325,7 +2310,7 @@
         <v>26</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -2360,7 +2345,7 @@
         <v>25</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2395,7 +2380,7 @@
         <v>25</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2430,7 +2415,7 @@
         <v>22</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2465,7 +2450,7 @@
         <v>22</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2500,7 +2485,7 @@
         <v>22</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2535,7 +2520,7 @@
         <v>25</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2570,7 +2555,7 @@
         <v>25</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -2605,7 +2590,7 @@
         <v>25</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -2640,7 +2625,7 @@
         <v>25</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2675,7 +2660,7 @@
         <v>25</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -2710,7 +2695,7 @@
         <v>25</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -2745,7 +2730,7 @@
         <v>25</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2780,7 +2765,7 @@
         <v>25</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -2815,7 +2800,7 @@
         <v>25</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -2850,7 +2835,7 @@
         <v>25</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2885,7 +2870,7 @@
         <v>25</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
@@ -2920,7 +2905,7 @@
         <v>25</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -2934,14 +2919,14 @@
         <v>6</v>
       </c>
       <c r="D54" s="4">
-        <f t="shared" ref="D54:D87" si="18">C54/B54</f>
+        <f t="shared" ref="D54:D82" si="18">C54/B54</f>
         <v>1.4944704593005878E-4</v>
       </c>
       <c r="E54" s="4">
         <v>14</v>
       </c>
       <c r="F54" s="4">
-        <f t="shared" ref="F54:F87" si="19">E54/B54</f>
+        <f t="shared" ref="F54:F82" si="19">E54/B54</f>
         <v>3.4870977383680382E-4</v>
       </c>
       <c r="G54" s="3">
@@ -2955,7 +2940,7 @@
         <v>25</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2990,7 +2975,7 @@
         <v>25</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -3025,7 +3010,7 @@
         <v>25</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -3060,7 +3045,7 @@
         <v>25</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -3095,7 +3080,7 @@
         <v>25</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3130,7 +3115,7 @@
         <v>25</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -3169,7 +3154,7 @@
         <v>31</v>
       </c>
       <c r="M60" s="64" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -3208,7 +3193,7 @@
         <v>31</v>
       </c>
       <c r="M61" s="64" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -3247,7 +3232,7 @@
         <v>31</v>
       </c>
       <c r="M62" s="64" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:13" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3286,7 +3271,7 @@
         <v>31</v>
       </c>
       <c r="M63" s="64" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -3325,7 +3310,7 @@
         <v>25</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -3364,7 +3349,7 @@
         <v>25</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -3403,7 +3388,7 @@
         <v>25</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -3442,7 +3427,7 @@
         <v>25</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3481,7 +3466,7 @@
         <v>25</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
@@ -3520,7 +3505,7 @@
         <v>22</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3559,693 +3544,498 @@
         <v>22</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A71" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B71" s="9">
-        <v>380</v>
-      </c>
-      <c r="C71" s="10">
-        <v>24</v>
-      </c>
-      <c r="D71" s="10">
-        <f t="shared" si="18"/>
-        <v>6.3157894736842107E-2</v>
-      </c>
-      <c r="E71" s="10">
-        <v>46</v>
-      </c>
-      <c r="F71" s="10">
-        <f t="shared" si="19"/>
-        <v>0.12105263157894737</v>
-      </c>
-      <c r="G71" s="9">
-        <v>2</v>
-      </c>
-      <c r="H71" s="10">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="I71" s="10">
-        <v>3.14</v>
-      </c>
-      <c r="J71" s="10"/>
-      <c r="K71" s="22"/>
-      <c r="L71" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B72" s="6">
-        <v>380</v>
-      </c>
-      <c r="C72" s="7">
-        <v>0</v>
-      </c>
-      <c r="D72" s="7">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="7">
-        <v>1</v>
-      </c>
-      <c r="F72" s="7">
-        <f t="shared" si="19"/>
-        <v>2.631578947368421E-3</v>
-      </c>
-      <c r="G72" s="6">
-        <v>2</v>
-      </c>
-      <c r="H72" s="7">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="I72" s="7">
-        <v>3.14</v>
-      </c>
-      <c r="J72" s="7"/>
-      <c r="K72" s="26"/>
-      <c r="L72" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A73" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B73" s="9">
-        <v>2147</v>
-      </c>
-      <c r="C73" s="10">
-        <v>408</v>
-      </c>
-      <c r="D73" s="10">
-        <f t="shared" si="18"/>
-        <v>0.19003260363297625</v>
-      </c>
-      <c r="E73" s="10">
-        <v>1024</v>
-      </c>
-      <c r="F73" s="10">
-        <f t="shared" si="19"/>
-        <v>0.4769445738239404</v>
-      </c>
-      <c r="G73" s="9">
-        <v>3</v>
-      </c>
-      <c r="H73" s="10">
-        <v>2.92</v>
-      </c>
-      <c r="I73" s="10">
-        <v>7.96</v>
-      </c>
-      <c r="J73" s="10"/>
-      <c r="K73" s="10"/>
-      <c r="L73" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A74" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B74" s="3">
-        <v>2147</v>
-      </c>
-      <c r="C74" s="4">
-        <v>3</v>
-      </c>
-      <c r="D74" s="4">
-        <f t="shared" si="18"/>
-        <v>1.3972985561248254E-3</v>
-      </c>
-      <c r="E74" s="4">
-        <v>6</v>
-      </c>
-      <c r="F74" s="4">
-        <f t="shared" si="19"/>
-        <v>2.7945971122496508E-3</v>
-      </c>
-      <c r="G74" s="3">
-        <v>3</v>
-      </c>
-      <c r="H74" s="4">
-        <v>2.92</v>
-      </c>
-      <c r="I74" s="4">
-        <v>7.96</v>
-      </c>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B75" s="6">
-        <v>2147</v>
-      </c>
-      <c r="C75" s="7">
-        <v>0</v>
-      </c>
-      <c r="D75" s="7">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E75" s="7">
-        <v>2</v>
-      </c>
-      <c r="F75" s="7">
-        <f t="shared" si="19"/>
-        <v>9.3153237074988359E-4</v>
-      </c>
-      <c r="G75" s="6">
-        <v>3</v>
-      </c>
-      <c r="H75" s="7">
-        <v>2.92</v>
-      </c>
-      <c r="I75" s="7">
-        <v>7.96</v>
-      </c>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B76" s="31">
+      <c r="B71" s="31">
         <v>4634</v>
       </c>
-      <c r="C76" s="32">
+      <c r="C71" s="32">
         <v>471</v>
       </c>
-      <c r="D76" s="32">
+      <c r="D71" s="32">
         <f t="shared" si="18"/>
         <v>0.10164005179110919</v>
       </c>
-      <c r="E76" s="32">
+      <c r="E71" s="32">
         <v>4571</v>
       </c>
-      <c r="F76" s="32">
+      <c r="F71" s="32">
         <f t="shared" si="19"/>
         <v>0.98640483383685795</v>
       </c>
-      <c r="G76" s="31">
+      <c r="G71" s="31">
         <v>7</v>
       </c>
-      <c r="H76" s="32">
+      <c r="H71" s="32">
         <v>21.81</v>
       </c>
-      <c r="I76" s="32">
+      <c r="I71" s="32">
         <v>11.42</v>
       </c>
-      <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
-      <c r="L76" s="34" t="s">
+      <c r="J71" s="32"/>
+      <c r="K71" s="32"/>
+      <c r="L71" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M76" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B77" s="37">
+      <c r="M71" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="37">
         <v>4634</v>
       </c>
-      <c r="C77" s="38">
+      <c r="C72" s="38">
         <v>514</v>
       </c>
-      <c r="D77" s="38">
+      <c r="D72" s="38">
         <f t="shared" si="18"/>
         <v>0.11091929218817437</v>
       </c>
-      <c r="E77" s="38">
+      <c r="E72" s="38">
         <v>2624</v>
       </c>
-      <c r="F77" s="38">
+      <c r="F72" s="38">
         <f t="shared" si="19"/>
         <v>0.56624946050927927</v>
       </c>
-      <c r="G77" s="37">
+      <c r="G72" s="37">
         <v>7</v>
       </c>
-      <c r="H77" s="38">
+      <c r="H72" s="38">
         <v>21.81</v>
       </c>
-      <c r="I77" s="38">
+      <c r="I72" s="38">
         <v>11.42</v>
       </c>
-      <c r="J77" s="38"/>
-      <c r="K77" s="38"/>
-      <c r="L77" s="40" t="s">
+      <c r="J72" s="38"/>
+      <c r="K72" s="38"/>
+      <c r="L72" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="M77" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B78" s="37">
+      <c r="M72" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="37">
         <v>4634</v>
       </c>
-      <c r="C78" s="38">
+      <c r="C73" s="38">
         <v>290</v>
       </c>
-      <c r="D78" s="38">
+      <c r="D73" s="38">
         <f t="shared" si="18"/>
         <v>6.2580923608113945E-2</v>
       </c>
-      <c r="E78" s="38">
+      <c r="E73" s="38">
         <v>1259</v>
       </c>
-      <c r="F78" s="38">
+      <c r="F73" s="38">
         <f t="shared" si="19"/>
         <v>0.27168752697453602</v>
       </c>
-      <c r="G78" s="37">
+      <c r="G73" s="37">
         <v>7</v>
       </c>
-      <c r="H78" s="38">
+      <c r="H73" s="38">
         <v>21.81</v>
       </c>
-      <c r="I78" s="38">
+      <c r="I73" s="38">
         <v>11.42</v>
       </c>
-      <c r="J78" s="38"/>
-      <c r="K78" s="38"/>
-      <c r="L78" s="40" t="s">
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
+      <c r="L73" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="M78" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B79" s="37">
+      <c r="M73" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" s="37">
         <v>4634</v>
       </c>
-      <c r="C79" s="38">
+      <c r="C74" s="38">
         <v>139</v>
       </c>
-      <c r="D79" s="38">
+      <c r="D74" s="38">
         <f t="shared" si="18"/>
         <v>2.9995684074233923E-2</v>
       </c>
-      <c r="E79" s="38">
+      <c r="E74" s="38">
         <v>540</v>
       </c>
-      <c r="F79" s="38">
+      <c r="F74" s="38">
         <f t="shared" si="19"/>
         <v>0.11652999568407424</v>
       </c>
-      <c r="G79" s="37">
+      <c r="G74" s="37">
         <v>7</v>
       </c>
-      <c r="H79" s="38">
+      <c r="H74" s="38">
         <v>21.81</v>
       </c>
-      <c r="I79" s="38">
+      <c r="I74" s="38">
         <v>11.42</v>
       </c>
-      <c r="J79" s="38"/>
-      <c r="K79" s="38"/>
-      <c r="L79" s="40" t="s">
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
+      <c r="L74" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="M79" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B80" s="37">
+      <c r="M74" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" s="37">
         <v>4634</v>
       </c>
-      <c r="C80" s="38">
+      <c r="C75" s="38">
         <v>23</v>
       </c>
-      <c r="D80" s="38">
+      <c r="D75" s="38">
         <f t="shared" si="18"/>
         <v>4.9633146309883474E-3</v>
       </c>
-      <c r="E80" s="38">
+      <c r="E75" s="38">
         <v>58</v>
       </c>
-      <c r="F80" s="38">
+      <c r="F75" s="38">
         <f t="shared" si="19"/>
         <v>1.2516184721622789E-2</v>
       </c>
-      <c r="G80" s="37">
+      <c r="G75" s="37">
         <v>7</v>
       </c>
-      <c r="H80" s="38">
+      <c r="H75" s="38">
         <v>21.81</v>
       </c>
-      <c r="I80" s="38">
+      <c r="I75" s="38">
         <v>11.42</v>
       </c>
-      <c r="J80" s="38"/>
-      <c r="K80" s="38"/>
-      <c r="L80" s="40" t="s">
+      <c r="J75" s="38"/>
+      <c r="K75" s="38"/>
+      <c r="L75" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="M80" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B81" s="37">
+      <c r="M75" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" s="37">
         <v>4634</v>
       </c>
-      <c r="C81" s="38">
+      <c r="C76" s="38">
         <v>2</v>
       </c>
-      <c r="D81" s="38">
+      <c r="D76" s="38">
         <f t="shared" si="18"/>
         <v>4.3159257660768235E-4</v>
       </c>
-      <c r="E81" s="38">
+      <c r="E76" s="38">
         <v>14</v>
       </c>
-      <c r="F81" s="38">
+      <c r="F76" s="38">
         <f t="shared" si="19"/>
         <v>3.0211480362537764E-3</v>
       </c>
-      <c r="G81" s="37">
+      <c r="G76" s="37">
         <v>7</v>
       </c>
-      <c r="H81" s="38">
+      <c r="H76" s="38">
         <v>21.81</v>
       </c>
-      <c r="I81" s="38">
+      <c r="I76" s="38">
         <v>11.42</v>
       </c>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
-      <c r="L81" s="40" t="s">
+      <c r="J76" s="38"/>
+      <c r="K76" s="38"/>
+      <c r="L76" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="M81" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B82" s="42">
+      <c r="M76" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="42">
         <v>4634</v>
       </c>
-      <c r="C82" s="43">
-        <v>0</v>
-      </c>
-      <c r="D82" s="43">
+      <c r="C77" s="43">
+        <v>0</v>
+      </c>
+      <c r="D77" s="43">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E82" s="43">
+      <c r="E77" s="43">
         <v>7</v>
       </c>
-      <c r="F82" s="43">
+      <c r="F77" s="43">
         <f t="shared" si="19"/>
         <v>1.5105740181268882E-3</v>
       </c>
-      <c r="G82" s="42">
+      <c r="G77" s="42">
         <v>7</v>
       </c>
-      <c r="H82" s="43">
+      <c r="H77" s="43">
         <v>21.81</v>
       </c>
-      <c r="I82" s="43">
+      <c r="I77" s="43">
         <v>11.42</v>
       </c>
-      <c r="J82" s="43"/>
-      <c r="K82" s="43"/>
-      <c r="L82" s="45" t="s">
+      <c r="J77" s="43"/>
+      <c r="K77" s="43"/>
+      <c r="L77" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="M82" s="64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="B83" s="52">
+      <c r="M77" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="52">
         <v>4432</v>
       </c>
-      <c r="C83" s="53">
+      <c r="C78" s="53">
         <v>42</v>
       </c>
-      <c r="D83" s="53">
+      <c r="D78" s="53">
         <f t="shared" si="18"/>
         <v>9.4765342960288802E-3</v>
       </c>
-      <c r="E83" s="53">
+      <c r="E78" s="53">
         <v>4432</v>
       </c>
-      <c r="F83" s="53">
+      <c r="F78" s="53">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="G83" s="52">
+      <c r="G78" s="52">
         <v>5</v>
       </c>
-      <c r="H83" s="53">
+      <c r="H78" s="53">
         <v>48.7</v>
       </c>
-      <c r="I83" s="53">
+      <c r="I78" s="53">
         <v>1961</v>
       </c>
-      <c r="J83" s="53">
+      <c r="J78" s="53">
         <v>1734</v>
       </c>
-      <c r="K83" s="53"/>
-      <c r="L83" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="M83" s="65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B84" s="57">
+      <c r="K78" s="53"/>
+      <c r="L78" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="M78" s="65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="57">
         <v>4432</v>
       </c>
-      <c r="C84" s="58">
+      <c r="C79" s="58">
         <v>16</v>
       </c>
-      <c r="D84" s="58">
+      <c r="D79" s="58">
         <f t="shared" si="18"/>
         <v>3.6101083032490976E-3</v>
       </c>
-      <c r="E84" s="58">
+      <c r="E79" s="58">
         <v>4344</v>
       </c>
-      <c r="F84" s="58">
+      <c r="F79" s="58">
         <f t="shared" si="19"/>
         <v>0.98014440433213001</v>
       </c>
-      <c r="G84" s="57">
+      <c r="G79" s="57">
         <v>5</v>
       </c>
-      <c r="H84" s="58">
+      <c r="H79" s="58">
         <v>48.7</v>
       </c>
-      <c r="I84" s="58">
+      <c r="I79" s="58">
         <v>1961</v>
       </c>
-      <c r="J84" s="58">
+      <c r="J79" s="58">
         <v>1734</v>
       </c>
-      <c r="K84" s="58"/>
-      <c r="L84" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="M84" s="65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B85" s="57">
+      <c r="K79" s="58"/>
+      <c r="L79" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="M79" s="65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" s="57">
         <v>4432</v>
       </c>
-      <c r="C85" s="58">
+      <c r="C80" s="58">
         <v>12</v>
       </c>
-      <c r="D85" s="58">
+      <c r="D80" s="58">
         <f t="shared" si="18"/>
         <v>2.707581227436823E-3</v>
       </c>
-      <c r="E85" s="58">
+      <c r="E80" s="58">
         <v>4310</v>
       </c>
-      <c r="F85" s="58">
+      <c r="F80" s="58">
         <f t="shared" si="19"/>
         <v>0.97247292418772568</v>
       </c>
-      <c r="G85" s="57">
+      <c r="G80" s="57">
         <v>5</v>
       </c>
-      <c r="H85" s="58">
+      <c r="H80" s="58">
         <v>48.7</v>
       </c>
-      <c r="I85" s="58">
+      <c r="I80" s="58">
         <v>1961</v>
       </c>
-      <c r="J85" s="58">
+      <c r="J80" s="58">
         <v>1734</v>
       </c>
-      <c r="K85" s="58"/>
-      <c r="L85" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="M85" s="65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B86" s="57">
+      <c r="K80" s="58"/>
+      <c r="L80" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="M80" s="65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" s="57">
         <v>4432</v>
       </c>
-      <c r="C86" s="58">
+      <c r="C81" s="58">
         <v>6</v>
       </c>
-      <c r="D86" s="58">
+      <c r="D81" s="58">
         <f t="shared" si="18"/>
         <v>1.3537906137184115E-3</v>
       </c>
-      <c r="E86" s="58">
+      <c r="E81" s="58">
         <v>4286</v>
       </c>
-      <c r="F86" s="58">
+      <c r="F81" s="58">
         <f t="shared" si="19"/>
         <v>0.96705776173285196</v>
       </c>
-      <c r="G86" s="57">
+      <c r="G81" s="57">
         <v>5</v>
       </c>
-      <c r="H86" s="58">
+      <c r="H81" s="58">
         <v>48.7</v>
       </c>
-      <c r="I86" s="58">
+      <c r="I81" s="58">
         <v>1961</v>
       </c>
-      <c r="J86" s="58">
+      <c r="J81" s="58">
         <v>1734</v>
       </c>
-      <c r="K86" s="58"/>
-      <c r="L86" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="M86" s="65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" s="55" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="B87" s="61">
+      <c r="K81" s="58"/>
+      <c r="L81" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="M81" s="65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="55" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" s="61">
         <v>4432</v>
       </c>
-      <c r="C87" s="62">
-        <v>0</v>
-      </c>
-      <c r="D87" s="62">
+      <c r="C82" s="62">
+        <v>0</v>
+      </c>
+      <c r="D82" s="62">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E87" s="62">
+      <c r="E82" s="62">
         <v>4274</v>
       </c>
-      <c r="F87" s="62">
+      <c r="F82" s="62">
         <f t="shared" si="19"/>
         <v>0.96435018050541521</v>
       </c>
-      <c r="G87" s="61">
+      <c r="G82" s="61">
         <v>5</v>
       </c>
-      <c r="H87" s="62">
+      <c r="H82" s="62">
         <v>48.7</v>
       </c>
-      <c r="I87" s="62">
+      <c r="I82" s="62">
         <v>1961</v>
       </c>
-      <c r="J87" s="62">
+      <c r="J82" s="62">
         <v>1734</v>
       </c>
-      <c r="K87" s="62"/>
-      <c r="L87" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="M87" s="65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
+      <c r="K82" s="62"/>
+      <c r="L82" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="M82" s="65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>